<commit_message>
Maps updated, gantt chart added, gantt chart dynamically shows individual sites
</commit_message>
<xml_diff>
--- a/data/SEACAR Program Matrix_ContinuousWQ_ProgramGroups.xlsx
+++ b/data/SEACAR Program Matrix_ContinuousWQ_ProgramGroups.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://floridadep-my.sharepoint.com/personal/tyler_hill_floridadep_gov/Documents/Desktop/SEACAR GitHub/SEACAR-Dashboards/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{A29DFB22-51D5-4278-A825-2870204128C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB6FA2C8-2A87-4170-9779-B8BB5851D46C}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="8_{A29DFB22-51D5-4278-A825-2870204128C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59A12A30-6424-4AB6-8DA1-49132CB1D281}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -356,16 +356,16 @@
     <t>Group</t>
   </si>
   <si>
-    <t>NERR SWMP</t>
-  </si>
-  <si>
-    <t>AP Continuous WQ Program</t>
-  </si>
-  <si>
     <t>Atlantic Oceanographic and Meteorological Laboratory (AOML) South Florida Program Moored Instrument Array</t>
   </si>
   <si>
     <t>Florida Keys National Marine Sanctuary Seagrass Monitoring Project</t>
+  </si>
+  <si>
+    <t>Aquatic Preserve Continuous Water Quality Program</t>
+  </si>
+  <si>
+    <t>National Estuarine Research Reserve SWMP</t>
   </si>
 </sst>
 </file>
@@ -767,7 +767,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,7 +848,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>13</v>
@@ -946,15 +946,15 @@
         <v>296</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>107</v>
+      <c r="A7" t="s">
+        <v>110</v>
       </c>
       <c r="B7" s="3">
         <v>354</v>
@@ -996,7 +996,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B8" s="3">
         <v>355</v>
@@ -1038,7 +1038,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B9" s="3">
         <v>467</v>
@@ -1079,8 +1079,8 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>108</v>
+      <c r="A10" s="5" t="s">
+        <v>109</v>
       </c>
       <c r="B10" s="3">
         <v>468</v>
@@ -1121,8 +1121,8 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>108</v>
+      <c r="A11" s="5" t="s">
+        <v>109</v>
       </c>
       <c r="B11" s="3">
         <v>471</v>
@@ -1163,8 +1163,8 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>108</v>
+      <c r="A12" s="5" t="s">
+        <v>109</v>
       </c>
       <c r="B12" s="3">
         <v>473</v>
@@ -1205,8 +1205,8 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>108</v>
+      <c r="A13" s="5" t="s">
+        <v>109</v>
       </c>
       <c r="B13" s="3">
         <v>474</v>
@@ -1286,8 +1286,8 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>108</v>
+      <c r="A15" s="5" t="s">
+        <v>109</v>
       </c>
       <c r="B15" s="3">
         <v>512</v>
@@ -1443,7 +1443,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B19" s="3">
         <v>4054</v>
@@ -1484,8 +1484,8 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>108</v>
+      <c r="A20" s="5" t="s">
+        <v>109</v>
       </c>
       <c r="B20" s="3">
         <v>5005</v>
@@ -1526,8 +1526,8 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>108</v>
+      <c r="A21" s="5" t="s">
+        <v>109</v>
       </c>
       <c r="B21" s="3">
         <v>5006</v>
@@ -1643,8 +1643,8 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>108</v>
+      <c r="A24" s="5" t="s">
+        <v>109</v>
       </c>
       <c r="B24" s="3">
         <v>5077</v>
@@ -1685,8 +1685,8 @@
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>108</v>
+      <c r="A25" s="5" t="s">
+        <v>109</v>
       </c>
       <c r="B25" s="3">
         <v>10003</v>

</xml_diff>

<commit_message>
applying SEACAR palette, working links
</commit_message>
<xml_diff>
--- a/data/SEACAR Program Matrix_ContinuousWQ_ProgramGroups.xlsx
+++ b/data/SEACAR Program Matrix_ContinuousWQ_ProgramGroups.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://floridadep-my.sharepoint.com/personal/tyler_hill_floridadep_gov/Documents/Desktop/SEACAR GitHub/SEACAR-Dashboards/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="8_{A29DFB22-51D5-4278-A825-2870204128C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59A12A30-6424-4AB6-8DA1-49132CB1D281}"/>
+  <xr:revisionPtr revIDLastSave="86" documentId="8_{A29DFB22-51D5-4278-A825-2870204128C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8EF2695B-568F-4059-96BA-B7DE57E0615B}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$25</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="133">
   <si>
     <t>SEACAR Program Matrix</t>
   </si>
@@ -356,23 +359,89 @@
     <t>Group</t>
   </si>
   <si>
-    <t>Atlantic Oceanographic and Meteorological Laboratory (AOML) South Florida Program Moored Instrument Array</t>
-  </si>
-  <si>
-    <t>Florida Keys National Marine Sanctuary Seagrass Monitoring Project</t>
-  </si>
-  <si>
     <t>Aquatic Preserve Continuous Water Quality Program</t>
   </si>
   <si>
     <t>National Estuarine Research Reserve SWMP</t>
+  </si>
+  <si>
+    <t>AOML South Florida Program Moored Instrument Array</t>
+  </si>
+  <si>
+    <t>FKNMS Seagrass Monitoring Project</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>https://data.florida-seacar.org/programs/details/5</t>
+  </si>
+  <si>
+    <t>https://data.florida-seacar.org/programs/details/7</t>
+  </si>
+  <si>
+    <t>https://data.florida-seacar.org/programs/details/354</t>
+  </si>
+  <si>
+    <t>https://data.florida-seacar.org/programs/details/355</t>
+  </si>
+  <si>
+    <t>https://data.florida-seacar.org/programs/details/467</t>
+  </si>
+  <si>
+    <t>https://data.florida-seacar.org/programs/details/468</t>
+  </si>
+  <si>
+    <t>https://data.florida-seacar.org/programs/details/471</t>
+  </si>
+  <si>
+    <t>https://data.florida-seacar.org/programs/details/473</t>
+  </si>
+  <si>
+    <t>https://data.florida-seacar.org/programs/details/474</t>
+  </si>
+  <si>
+    <t>https://data.florida-seacar.org/programs/details/505</t>
+  </si>
+  <si>
+    <t>https://data.florida-seacar.org/programs/details/512</t>
+  </si>
+  <si>
+    <t>https://data.florida-seacar.org/programs/details/912</t>
+  </si>
+  <si>
+    <t>https://data.florida-seacar.org/programs/details/986</t>
+  </si>
+  <si>
+    <t>https://data.florida-seacar.org/programs/details/989</t>
+  </si>
+  <si>
+    <t>https://data.florida-seacar.org/programs/details/4054</t>
+  </si>
+  <si>
+    <t>https://data.florida-seacar.org/programs/details/5005</t>
+  </si>
+  <si>
+    <t>https://data.florida-seacar.org/programs/details/5006</t>
+  </si>
+  <si>
+    <t>https://data.florida-seacar.org/programs/details/5061</t>
+  </si>
+  <si>
+    <t>https://data.florida-seacar.org/programs/details/5062</t>
+  </si>
+  <si>
+    <t>https://data.florida-seacar.org/programs/details/5077</t>
+  </si>
+  <si>
+    <t>https://data.florida-seacar.org/programs/details/10003</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -398,6 +467,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -416,22 +491,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -764,16 +842,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" customWidth="1"/>
+    <col min="1" max="1" width="47.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
     <col min="3" max="3" width="104.140625" customWidth="1"/>
     <col min="4" max="4" width="18.140625" customWidth="1"/>
     <col min="5" max="6" width="52" customWidth="1"/>
@@ -781,27 +859,28 @@
     <col min="8" max="8" width="10.42578125" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
     <col min="10" max="10" width="52" customWidth="1"/>
-    <col min="11" max="11" width="39" customWidth="1"/>
+    <col min="11" max="11" width="21.28515625" customWidth="1"/>
     <col min="12" max="13" width="52" customWidth="1"/>
+    <col min="14" max="14" width="36.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B1" s="6" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>106</v>
       </c>
@@ -841,14 +920,17 @@
       <c r="M2" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="5">
         <v>2</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>13</v>
@@ -862,8 +944,9 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3" s="5"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4" s="3">
         <v>5</v>
       </c>
@@ -901,8 +984,11 @@
       <c r="M4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
         <v>7</v>
       </c>
@@ -940,28 +1026,32 @@
       <c r="M5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N5" s="6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
         <v>296</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N6" s="2"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B7" s="3">
         <v>354</v>
       </c>
-      <c r="C7" s="2" t="str">
-        <f>HYPERLINK("https://data.florida-seacar.org/programs/details/354","Rookery Bay National Estuarine Research Reserve System-Wide Monitoring Program")</f>
-        <v>Rookery Bay National Estuarine Research Reserve System-Wide Monitoring Program</v>
+      <c r="C7" s="6" t="str">
+        <f>HYPERLINK("https://data.florida-seacar.org/programs/details/354","Rookery Bay National Estuarine Research Reserve SWMP")</f>
+        <v>Rookery Bay National Estuarine Research Reserve SWMP</v>
       </c>
       <c r="D7" t="s">
         <v>29</v>
@@ -993,17 +1083,20 @@
       <c r="M7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N7" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B8" s="3">
         <v>355</v>
       </c>
-      <c r="C8" s="2" t="str">
-        <f>HYPERLINK("https://data.florida-seacar.org/programs/details/355","Apalachicola National Estuarine Research Reserve System-Wide Monitoring Program")</f>
-        <v>Apalachicola National Estuarine Research Reserve System-Wide Monitoring Program</v>
+      <c r="C8" s="6" t="str">
+        <f>HYPERLINK("https://data.florida-seacar.org/programs/details/355","Apalachicola National Estuarine Research Reserve SWMP")</f>
+        <v>Apalachicola National Estuarine Research Reserve SWMP</v>
       </c>
       <c r="D8" t="s">
         <v>34</v>
@@ -1035,17 +1128,20 @@
       <c r="M8" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N8" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B9" s="3">
         <v>467</v>
       </c>
-      <c r="C9" s="2" t="str">
-        <f>HYPERLINK("https://data.florida-seacar.org/programs/details/467","Yellow River Marsh Aquatic Preserve Continuous Water Quality Monitoring")</f>
-        <v>Yellow River Marsh Aquatic Preserve Continuous Water Quality Monitoring</v>
+      <c r="C9" s="6" t="str">
+        <f>HYPERLINK("https://data.florida-seacar.org/programs/details/467","Yellow River Marsh Aquatic Preserve")</f>
+        <v>Yellow River Marsh Aquatic Preserve</v>
       </c>
       <c r="D9" t="s">
         <v>34</v>
@@ -1077,17 +1173,20 @@
       <c r="M9" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N9" s="6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B10" s="3">
         <v>468</v>
       </c>
-      <c r="C10" s="2" t="str">
-        <f>HYPERLINK("https://data.florida-seacar.org/programs/details/468","Central Panhandle Aquatic Preserves Continuous Water Quality Monitoring")</f>
-        <v>Central Panhandle Aquatic Preserves Continuous Water Quality Monitoring</v>
+      <c r="C10" s="6" t="str">
+        <f>HYPERLINK("https://data.florida-seacar.org/programs/details/468","Central Panhandle Aquatic Preserves")</f>
+        <v>Central Panhandle Aquatic Preserves</v>
       </c>
       <c r="D10" t="s">
         <v>34</v>
@@ -1119,17 +1218,20 @@
       <c r="M10" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N10" s="6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B11" s="3">
         <v>471</v>
       </c>
-      <c r="C11" s="2" t="str">
-        <f>HYPERLINK("https://data.florida-seacar.org/programs/details/471","Big Bend Seagrasses Aquatic Preserves Continuous Water Quality Monitoring")</f>
-        <v>Big Bend Seagrasses Aquatic Preserves Continuous Water Quality Monitoring</v>
+      <c r="C11" s="6" t="str">
+        <f>HYPERLINK("https://data.florida-seacar.org/programs/details/471","Big Bend Seagrasses Aquatic Preserves")</f>
+        <v>Big Bend Seagrasses Aquatic Preserves</v>
       </c>
       <c r="D11" t="s">
         <v>34</v>
@@ -1161,17 +1263,20 @@
       <c r="M11" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N11" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B12" s="3">
         <v>473</v>
       </c>
-      <c r="C12" s="2" t="str">
-        <f>HYPERLINK("https://data.florida-seacar.org/programs/details/473","Terra Ceia Aquatic Preserve Continuous Water Quality Monitoring")</f>
-        <v>Terra Ceia Aquatic Preserve Continuous Water Quality Monitoring</v>
+      <c r="C12" s="6" t="str">
+        <f>HYPERLINK("https://data.florida-seacar.org/programs/details/473","Terra Ceia Aquatic Preserve")</f>
+        <v>Terra Ceia Aquatic Preserve</v>
       </c>
       <c r="D12" t="s">
         <v>29</v>
@@ -1203,17 +1308,20 @@
       <c r="M12" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N12" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B13" s="3">
         <v>474</v>
       </c>
-      <c r="C13" s="2" t="str">
-        <f>HYPERLINK("https://data.florida-seacar.org/programs/details/474","Estero Bay Aquatic Preserve Continuous Water Quality Monitoring")</f>
-        <v>Estero Bay Aquatic Preserve Continuous Water Quality Monitoring</v>
+      <c r="C13" s="6" t="str">
+        <f>HYPERLINK("https://data.florida-seacar.org/programs/details/474","Estero Bay Aquatic Preserve")</f>
+        <v>Estero Bay Aquatic Preserve</v>
       </c>
       <c r="D13" t="s">
         <v>29</v>
@@ -1245,14 +1353,17 @@
       <c r="M13" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N13" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <v>505</v>
       </c>
-      <c r="C14" s="2" t="str">
-        <f>HYPERLINK("https://data.florida-seacar.org/programs/details/505","Pensacola Bay Water Quality Monitoring Program")</f>
-        <v>Pensacola Bay Water Quality Monitoring Program</v>
+      <c r="C14" s="6" t="str">
+        <f>HYPERLINK("https://data.florida-seacar.org/programs/details/505","Pensacola Bay WQ Monitoring Program")</f>
+        <v>Pensacola Bay WQ Monitoring Program</v>
       </c>
       <c r="D14" t="s">
         <v>34</v>
@@ -1284,17 +1395,20 @@
       <c r="M14" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N14" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B15" s="3">
         <v>512</v>
       </c>
-      <c r="C15" s="2" t="str">
-        <f>HYPERLINK("https://data.florida-seacar.org/programs/details/512","Charlotte Harbor Aquatic Preserves Continuous Water Quality Monitoring Program")</f>
-        <v>Charlotte Harbor Aquatic Preserves Continuous Water Quality Monitoring Program</v>
+      <c r="C15" s="6" t="str">
+        <f>HYPERLINK("https://data.florida-seacar.org/programs/details/512","Charlotte Harbor Aquatic Preserves")</f>
+        <v>Charlotte Harbor Aquatic Preserves</v>
       </c>
       <c r="D15" t="s">
         <v>29</v>
@@ -1326,12 +1440,15 @@
       <c r="M15" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N15" s="6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <v>912</v>
       </c>
-      <c r="C16" s="2" t="str">
+      <c r="C16" s="6" t="str">
         <f>HYPERLINK("https://data.florida-seacar.org/programs/details/912","NPS South Florida/Caribbean Inventory and Monitoring Network: Coral Reef Water Temperature")</f>
         <v>NPS South Florida/Caribbean Inventory and Monitoring Network: Coral Reef Water Temperature</v>
       </c>
@@ -1362,8 +1479,11 @@
       <c r="L16" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N16" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <v>986</v>
       </c>
@@ -1401,8 +1521,11 @@
       <c r="M17" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N17" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <v>989</v>
       </c>
@@ -1440,17 +1563,20 @@
       <c r="M18" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N18" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B19" s="3">
         <v>4054</v>
       </c>
-      <c r="C19" s="2" t="str">
-        <f>HYPERLINK("https://data.florida-seacar.org/programs/details/4054","Guana Tolomato Matanzas National Estuarine Research Reserve System-Wide Monitoring Program")</f>
-        <v>Guana Tolomato Matanzas National Estuarine Research Reserve System-Wide Monitoring Program</v>
+      <c r="C19" s="6" t="str">
+        <f>HYPERLINK("https://data.florida-seacar.org/programs/details/4054","Guana Tolomato Matanzas National Estuarine Research Reserve SWMP")</f>
+        <v>Guana Tolomato Matanzas National Estuarine Research Reserve SWMP</v>
       </c>
       <c r="D19" t="s">
         <v>79</v>
@@ -1482,17 +1608,20 @@
       <c r="M19" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N19" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B20" s="3">
         <v>5005</v>
       </c>
-      <c r="C20" s="2" t="str">
-        <f>HYPERLINK("https://data.florida-seacar.org/programs/details/5005","Indian River Lagoon Aquatic Preserves Continuous Water Quality Monitoring")</f>
-        <v>Indian River Lagoon Aquatic Preserves Continuous Water Quality Monitoring</v>
+      <c r="C20" s="6" t="str">
+        <f>HYPERLINK("https://data.florida-seacar.org/programs/details/5005","Indian River Lagoon Aquatic Preserves")</f>
+        <v>Indian River Lagoon Aquatic Preserves</v>
       </c>
       <c r="D20" t="s">
         <v>79</v>
@@ -1524,17 +1653,20 @@
       <c r="M20" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N20" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B21" s="3">
         <v>5006</v>
       </c>
-      <c r="C21" s="2" t="str">
-        <f>HYPERLINK("https://data.florida-seacar.org/programs/details/5006","Northeast Aquatic Preserves Continuous Water Quality Monitoring")</f>
-        <v>Northeast Aquatic Preserves Continuous Water Quality Monitoring</v>
+      <c r="C21" s="6" t="str">
+        <f>HYPERLINK("https://data.florida-seacar.org/programs/details/5006","Northeast Aquatic Preserves")</f>
+        <v>Northeast Aquatic Preserves</v>
       </c>
       <c r="D21" t="s">
         <v>79</v>
@@ -1566,14 +1698,17 @@
       <c r="M21" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N21" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <v>5061</v>
       </c>
-      <c r="C22" s="2" t="str">
-        <f>HYPERLINK("https://data.florida-seacar.org/programs/details/5061","St. Johns River Water Management District Continuous Water Quality Programs")</f>
-        <v>St. Johns River Water Management District Continuous Water Quality Programs</v>
+      <c r="C22" s="6" t="str">
+        <f>HYPERLINK("https://data.florida-seacar.org/programs/details/5061","St. Johns River Water Management District Continuous WQ Programs")</f>
+        <v>St. Johns River Water Management District Continuous WQ Programs</v>
       </c>
       <c r="D22" t="s">
         <v>79</v>
@@ -1602,14 +1737,17 @@
       <c r="M22" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N22" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <v>5062</v>
       </c>
-      <c r="C23" s="2" t="str">
-        <f>HYPERLINK("https://data.florida-seacar.org/programs/details/5062","FDEP Bureau of Survey and Mapping Continuous Water Quality Program")</f>
-        <v>FDEP Bureau of Survey and Mapping Continuous Water Quality Program</v>
+      <c r="C23" s="6" t="str">
+        <f>HYPERLINK("https://data.florida-seacar.org/programs/details/5062","FDEP Bureau of Survey and Mapping Continuous WQ Program")</f>
+        <v>FDEP Bureau of Survey and Mapping Continuous WQ Program</v>
       </c>
       <c r="D23" t="s">
         <v>94</v>
@@ -1641,17 +1779,20 @@
       <c r="M23" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N23" s="6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B24" s="3">
         <v>5077</v>
       </c>
-      <c r="C24" s="2" t="str">
-        <f>HYPERLINK("https://data.florida-seacar.org/programs/details/5077","Biscayne Bay Aquatic Preserves Continuous Water Quality Monitoring")</f>
-        <v>Biscayne Bay Aquatic Preserves Continuous Water Quality Monitoring</v>
+      <c r="C24" s="6" t="str">
+        <f>HYPERLINK("https://data.florida-seacar.org/programs/details/5077","Biscayne Bay Aquatic Preserves")</f>
+        <v>Biscayne Bay Aquatic Preserves</v>
       </c>
       <c r="D24" t="s">
         <v>13</v>
@@ -1683,17 +1824,20 @@
       <c r="M24" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N24" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B25" s="3">
         <v>10003</v>
       </c>
-      <c r="C25" s="2" t="str">
-        <f>HYPERLINK("https://data.florida-seacar.org/programs/details/10003","Tomoka Marsh Aquatic Preserve Continuous Water Quality Monitoring")</f>
-        <v>Tomoka Marsh Aquatic Preserve Continuous Water Quality Monitoring</v>
+      <c r="C25" s="6" t="str">
+        <f>HYPERLINK("https://data.florida-seacar.org/programs/details/10003","Tomoka Marsh Aquatic Preserve")</f>
+        <v>Tomoka Marsh Aquatic Preserve</v>
       </c>
       <c r="D25" t="s">
         <v>79</v>
@@ -1725,11 +1869,50 @@
       <c r="M25" t="s">
         <v>105</v>
       </c>
+      <c r="N25" s="6" t="s">
+        <v>132</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:M25" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="1" showButton="0"/>
+    <filterColumn colId="2" showButton="0"/>
+    <filterColumn colId="3" showButton="0"/>
+    <filterColumn colId="4" showButton="0"/>
+    <filterColumn colId="5" showButton="0"/>
+    <filterColumn colId="6" showButton="0"/>
+    <filterColumn colId="7" showButton="0"/>
+    <filterColumn colId="8" showButton="0"/>
+    <filterColumn colId="9" showButton="0"/>
+    <filterColumn colId="10" showButton="0"/>
+    <filterColumn colId="11" showButton="0"/>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="B1:M1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="N4" r:id="rId1" xr:uid="{6323A6E5-19FA-4BEB-BAE9-EDFA836AC8D0}"/>
+    <hyperlink ref="N5" r:id="rId2" xr:uid="{7FE57FCD-C9ED-4412-8AC9-FB24CE01AB71}"/>
+    <hyperlink ref="N7" r:id="rId3" xr:uid="{02AFF292-4497-4A9A-86F4-4BF4AB64CFA3}"/>
+    <hyperlink ref="N8" r:id="rId4" xr:uid="{26F6B38D-99AB-461D-BAA6-E1FBBBA9ABD1}"/>
+    <hyperlink ref="N9" r:id="rId5" xr:uid="{EA076D0F-E5C7-42F1-BC9B-915F3A0DD499}"/>
+    <hyperlink ref="N10" r:id="rId6" xr:uid="{2A66CC86-345D-494C-87DA-5369563F39ED}"/>
+    <hyperlink ref="N11" r:id="rId7" xr:uid="{5474AEBC-259D-41AD-863E-5EA3CB0A1AB3}"/>
+    <hyperlink ref="N12" r:id="rId8" xr:uid="{483EFD26-DB37-4C0E-8ECB-5D8E598463D5}"/>
+    <hyperlink ref="N13" r:id="rId9" xr:uid="{277B51B8-4681-4BD7-819A-6470AB010DC1}"/>
+    <hyperlink ref="N14" r:id="rId10" xr:uid="{FF04700F-6E20-4AB2-9CCE-E636D5F1246B}"/>
+    <hyperlink ref="N15" r:id="rId11" xr:uid="{B54271DA-D6B8-48B0-ABED-1579F770B409}"/>
+    <hyperlink ref="N16" r:id="rId12" xr:uid="{0B6F7558-D118-4DA6-B351-B0487CAEBA85}"/>
+    <hyperlink ref="N17" r:id="rId13" xr:uid="{84726E89-63E9-4999-9E99-EDC19A4363CF}"/>
+    <hyperlink ref="N18" r:id="rId14" xr:uid="{8793E51B-6A32-4EA0-9431-97A7CFB79FB3}"/>
+    <hyperlink ref="N19" r:id="rId15" xr:uid="{1AE4789C-B69E-4FF3-967C-6B064A48C76D}"/>
+    <hyperlink ref="N20" r:id="rId16" xr:uid="{68EAE73E-B00B-47D3-A3A3-B0ACF1A7E258}"/>
+    <hyperlink ref="N21" r:id="rId17" xr:uid="{83575383-3AEC-4889-8CAB-CE18F3CF8C6A}"/>
+    <hyperlink ref="N22" r:id="rId18" xr:uid="{FDDE9BBA-CE2C-4DAD-A2DC-D54F3461346D}"/>
+    <hyperlink ref="N23" r:id="rId19" xr:uid="{5B11E175-41D8-4085-AF02-625CA505F67B}"/>
+    <hyperlink ref="N24" r:id="rId20" xr:uid="{8DFAEE79-5FBA-4BAF-A64D-D55C07A5112B}"/>
+    <hyperlink ref="N25" r:id="rId21" xr:uid="{8D88C2A4-CCFA-4238-A14D-6A4667C58823}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>